<commit_message>
New DELRTE command, DELRTE KL204 now deletes entire route incl dest and orig Synonyms also used in radarclick Docs updated
</commit_message>
<xml_diff>
--- a/docs/BLUESKY-COMMAND-TABLE.xlsx
+++ b/docs/BLUESKY-COMMAND-TABLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="390">
   <si>
     <t>Command</t>
   </si>
@@ -241,9 +241,6 @@
     <t>txt,[latlon,txt,txt,txt]</t>
   </si>
   <si>
-    <t xml:space="preserve"> Navdatabase.defwpt of bluesky.navdb.navdb.Navdatabase instance</t>
-  </si>
-  <si>
     <t>DEL</t>
   </si>
   <si>
@@ -1171,7 +1168,22 @@
     <t>VRESOMETH</t>
   </si>
   <si>
-    <t>Define a new waypoint for this scenario</t>
+    <t>Define a waypoint only for this scenario/run</t>
+  </si>
+  <si>
+    <t>DELRTE</t>
+  </si>
+  <si>
+    <t>Delete for this a/c the complete route/dest/orig (FMS)</t>
+  </si>
+  <si>
+    <t>DELRTE acid</t>
+  </si>
+  <si>
+    <t>HEADING</t>
+  </si>
+  <si>
+    <t>SPEED</t>
   </si>
 </sst>
 </file>
@@ -2036,10 +2048,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2326,7 @@
         <v>71</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>73</v>
@@ -2322,1172 +2334,1185 @@
       <c r="D17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>80</v>
+        <v>385</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>386</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>81</v>
+        <v>387</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>99</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>120</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E36" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="2" t="s">
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>177</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E42" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>190</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E45" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>197</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D49" s="2"/>
+        <v>203</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="E49" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>236</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D57" s="2"/>
+        <v>233</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="E57" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E67" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E69" s="2" t="s">
-        <v>284</v>
-      </c>
+      <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D73" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E73" s="2" t="s">
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D75" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E74" s="2" t="s">
+    </row>
+    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="E75" s="2" t="s">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C77" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2" t="s">
+    </row>
+    <row r="78" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E77" s="2"/>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>320</v>
-      </c>
+      <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D80" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>176</v>
+        <v>327</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="E82" s="2" t="s">
+    </row>
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="E84" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E86" s="2"/>
+      <c r="E87" s="2"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
     <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>62</v>
@@ -3498,266 +3523,288 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>259</v>
+        <v>140</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>260</v>
+        <v>141</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>152</v>
+        <v>258</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>153</v>
+        <v>259</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C106" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>141</v>
+        <v>205</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>142</v>
+        <v>206</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>263</v>
+        <v>140</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>264</v>
+        <v>141</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B118" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>264</v>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>